<commit_message>
Atualizacao da Page, inserindo Assert para teste positivo e negativo
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641DA51D-DDF1-488F-847C-17C9B32160BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A890B3-4E2D-4206-93E0-B94A486502E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>campoApelido</t>
   </si>
@@ -101,7 +101,43 @@
     <t>16060-380</t>
   </si>
   <si>
-    <t>Wilkerbn007</t>
+    <t>Wilkerbn010</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>HP PAVILION 15T TOUCH LAPTOP</t>
+  </si>
+  <si>
+    <t>LAPTOPS</t>
+  </si>
+  <si>
+    <t>campoCategoria(Pesquisa)</t>
+  </si>
+  <si>
+    <t>campoProduto (Pesquisa)</t>
+  </si>
+  <si>
+    <t>campoCategoria(Tela Principal)</t>
+  </si>
+  <si>
+    <t>campoProduto (Tela Principal)</t>
+  </si>
+  <si>
+    <t>HP Pavilion 15z Laptop</t>
+  </si>
+  <si>
+    <t>produtoInvalido</t>
+  </si>
+  <si>
+    <t>Video Game</t>
+  </si>
+  <si>
+    <t>ResultadoDoProdutoInvalido</t>
+  </si>
+  <si>
+    <t>No results for "Video Game"</t>
   </si>
 </sst>
 </file>
@@ -467,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98928E84-822C-4435-A3C7-42A4956E9C7D}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,10 +523,15 @@
     <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +568,26 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -564,6 +623,24 @@
       </c>
       <c r="L2" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizacao de Asserts e implementacao de screenshots
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A890B3-4E2D-4206-93E0-B94A486502E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06860ADC-3C02-4D0B-BFFF-5634C7E6EA27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>campoApelido</t>
   </si>
@@ -101,9 +101,6 @@
     <t>16060-380</t>
   </si>
   <si>
-    <t>Wilkerbn010</t>
-  </si>
-  <si>
     <t>Laptop</t>
   </si>
   <si>
@@ -138,13 +135,34 @@
   </si>
   <si>
     <t>No results for "Video Game"</t>
+  </si>
+  <si>
+    <t>resultadoCadastroDuplicado</t>
+  </si>
+  <si>
+    <t>User name already exists</t>
+  </si>
+  <si>
+    <t>HP PAVILION 15Z LAPTOP</t>
+  </si>
+  <si>
+    <t>produtoValidoEsperado</t>
+  </si>
+  <si>
+    <t>Oops! We only have 10 in stock. We updated your order accordingly</t>
+  </si>
+  <si>
+    <t>comparaQuantidadeInvalidaDeProdutosTelaPrincipal</t>
+  </si>
+  <si>
+    <t>Wilkerbn013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,13 +178,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,12 +214,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -503,16 +536,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98928E84-822C-4435-A3C7-42A4956E9C7D}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
@@ -529,67 +562,71 @@
     <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
+      <c r="Q1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -625,22 +662,41 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -648,5 +704,6 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{FC2525D2-361F-4438-89AD-1D1DB66A512C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização Excel e parametrização, atualização de comandos de espera
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06860ADC-3C02-4D0B-BFFF-5634C7E6EA27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539FE9B0-4FD0-4AB3-A40D-252B596B1493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
+    <sheet name="Produtos" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,43 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
-  <si>
-    <t>campoApelido</t>
-  </si>
-  <si>
-    <t>campoSenha</t>
-  </si>
-  <si>
-    <t>campoConfirmaSenha</t>
-  </si>
-  <si>
-    <t>campoEmail</t>
-  </si>
-  <si>
-    <t>campoPrimeiroNome</t>
-  </si>
-  <si>
-    <t>campoUltimoNome</t>
-  </si>
-  <si>
-    <t>campoTelefone</t>
-  </si>
-  <si>
-    <t>campoPais</t>
-  </si>
-  <si>
-    <t>campoCidade</t>
-  </si>
-  <si>
-    <t>campoEndereco</t>
-  </si>
-  <si>
-    <t>campoEstado</t>
-  </si>
-  <si>
-    <t>campoCep</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>Wbn221190</t>
   </si>
@@ -110,59 +76,227 @@
     <t>LAPTOPS</t>
   </si>
   <si>
-    <t>campoCategoria(Pesquisa)</t>
-  </si>
-  <si>
-    <t>campoProduto (Pesquisa)</t>
-  </si>
-  <si>
-    <t>campoCategoria(Tela Principal)</t>
-  </si>
-  <si>
-    <t>campoProduto (Tela Principal)</t>
-  </si>
-  <si>
     <t>HP Pavilion 15z Laptop</t>
   </si>
   <si>
-    <t>produtoInvalido</t>
-  </si>
-  <si>
     <t>Video Game</t>
   </si>
   <si>
-    <t>ResultadoDoProdutoInvalido</t>
-  </si>
-  <si>
     <t>No results for "Video Game"</t>
   </si>
   <si>
-    <t>resultadoCadastroDuplicado</t>
-  </si>
-  <si>
     <t>User name already exists</t>
   </si>
   <si>
     <t>HP PAVILION 15Z LAPTOP</t>
   </si>
   <si>
-    <t>produtoValidoEsperado</t>
-  </si>
-  <si>
     <t>Oops! We only have 10 in stock. We updated your order accordingly</t>
   </si>
   <si>
-    <t>comparaQuantidadeInvalidaDeProdutosTelaPrincipal</t>
-  </si>
-  <si>
-    <t>Wilkerbn013</t>
+    <t>Wilkerbn015</t>
+  </si>
+  <si>
+    <t>campoApelido (1,0)</t>
+  </si>
+  <si>
+    <t>campoSenha (1,1)</t>
+  </si>
+  <si>
+    <t>campoConfirmaSenha (1,2)</t>
+  </si>
+  <si>
+    <t>campoEmail (1,3)</t>
+  </si>
+  <si>
+    <t>campoPrimeiroNome (1,4)</t>
+  </si>
+  <si>
+    <t>campoUltimoNome (1,5)</t>
+  </si>
+  <si>
+    <t>campoTelefone (1,6)</t>
+  </si>
+  <si>
+    <t>campoPais (1,7)</t>
+  </si>
+  <si>
+    <t>campoCidade (1,8)</t>
+  </si>
+  <si>
+    <t>campoEndereco (1,9)</t>
+  </si>
+  <si>
+    <t>campoEstado (1,10)</t>
+  </si>
+  <si>
+    <t>campoCep (1,11)</t>
+  </si>
+  <si>
+    <t>campoCategoria - Lupa (1,12)</t>
+  </si>
+  <si>
+    <t>campoProduto - Lupa (1,13)</t>
+  </si>
+  <si>
+    <t>campoCategoria - Tela Principal (1,14)</t>
+  </si>
+  <si>
+    <t>campoProduto - Tela Principal (1,15)</t>
+  </si>
+  <si>
+    <t>produtoInvalido (1,16)</t>
+  </si>
+  <si>
+    <t>ResultadoDoProdutoInvalido (1,17)</t>
+  </si>
+  <si>
+    <t>resultadoCadastroDuplicado (1,18)</t>
+  </si>
+  <si>
+    <t>produtoValidoEsperado (4,0)</t>
+  </si>
+  <si>
+    <t>comparaQuantidadeInvalidaDeProdutosTelaPrincipal (4,1)</t>
+  </si>
+  <si>
+    <t>Usuaria Já utilizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apelido </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senha  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmar Senha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primeiro Nome </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultimo Nome </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">País </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cidade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endereço </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cep </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posição </t>
+  </si>
+  <si>
+    <t>Cenário Formulário de Cadastro</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Produtos Validos</t>
+  </si>
+  <si>
+    <t>mice</t>
+  </si>
+  <si>
+    <t>headphones</t>
+  </si>
+  <si>
+    <t>laptops</t>
+  </si>
+  <si>
+    <t>Validação</t>
+  </si>
+  <si>
+    <t>Posição</t>
+  </si>
+  <si>
+    <t>Logitech USB Headset H390</t>
+  </si>
+  <si>
+    <t>LOGITECH USB HEADSET H390</t>
+  </si>
+  <si>
+    <t>HP Z3600 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>HP Z3600 WIRELESS MOUSE</t>
+  </si>
+  <si>
+    <t>HP ENVY x360 - 15t Laptop</t>
+  </si>
+  <si>
+    <t>HP ENVY X360 - 15T LAPTOP</t>
+  </si>
+  <si>
+    <t>C(2,0) P(2,1) V(2,2)</t>
+  </si>
+  <si>
+    <t>C(3,0) P(3,1) V(3,2)</t>
+  </si>
+  <si>
+    <t>C(4,0) P(4,1) V(4,2)</t>
+  </si>
+  <si>
+    <t>Produtos Inexistentes</t>
+  </si>
+  <si>
+    <t>Televisão</t>
+  </si>
+  <si>
+    <t>No results for "Televisão"</t>
+  </si>
+  <si>
+    <t>Apartamento</t>
+  </si>
+  <si>
+    <t>No results for "Apartamento"</t>
+  </si>
+  <si>
+    <t>P(12,0) V(12,1)</t>
+  </si>
+  <si>
+    <t>P(13,0) V(13,1)</t>
+  </si>
+  <si>
+    <t>P(11,0) V(11,1)</t>
+  </si>
+  <si>
+    <t>Wilkerbn22</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Q(7,0) V(7,1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +320,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,12 +344,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,18 +387,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -538,165 +759,165 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98928E84-822C-4435-A3C7-42A4956E9C7D}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -706,4 +927,345 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05728C-6319-46C4-B137-F84177D05307}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="11">
+        <v>13.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{43081A23-0928-4EAE-B817-FE98168EC0D3}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F037193-F877-43F4-BA53-AC2F28E12A40}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:C10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização de projeto, ajustes.
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539FE9B0-4FD0-4AB3-A40D-252B596B1493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C44DDAE-1E51-4A7F-BF73-89546CEF5FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -274,22 +274,22 @@
     <t>No results for "Apartamento"</t>
   </si>
   <si>
-    <t>P(12,0) V(12,1)</t>
-  </si>
-  <si>
-    <t>P(13,0) V(13,1)</t>
-  </si>
-  <si>
-    <t>P(11,0) V(11,1)</t>
-  </si>
-  <si>
-    <t>Wilkerbn22</t>
-  </si>
-  <si>
     <t>999</t>
   </si>
   <si>
     <t>Q(7,0) V(7,1)</t>
+  </si>
+  <si>
+    <t>C(11,0) V(11,1)</t>
+  </si>
+  <si>
+    <t>C(12,0) V(12,1)</t>
+  </si>
+  <si>
+    <t>C(13,0) V(13,1)</t>
+  </si>
+  <si>
+    <t>Wilkerbn504</t>
   </si>
 </sst>
 </file>
@@ -430,6 +430,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,9 +441,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05728C-6319-46C4-B137-F84177D05307}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -945,10 +945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="10" t="s">
         <v>54</v>
       </c>
@@ -958,7 +958,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" s="11">
         <v>1.1000000000000001</v>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F037193-F877-43F4-BA53-AC2F28E12A40}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,12 +1125,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -1200,22 +1200,22 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>83</v>
+      <c r="A8" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -1247,7 +1247,7 @@
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
         <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do caminho relativo, adicionado chromedriver na pasta do projeto, classe para consulta de arquivos json adicionada.
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF8DF02-04C4-41A3-8879-E828125C5618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FF7CF4-1C34-4C0C-B4C4-A64A17598676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -289,7 +289,7 @@
     <t>C(13,0) V(13,1)</t>
   </si>
   <si>
-    <t>Wilkerbn801</t>
+    <t>Wilkerbn815</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Alteração caminho relativo e driver
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/tdd/testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace\avaliacao-automacao-tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-avaliacao-final\Avaliacao-Rsi-Automacao-Tdd\src\test\java\br\com\rsinet\hub\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FF7CF4-1C34-4C0C-B4C4-A64A17598676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79CEDC3-35EE-4762-A6AB-5AD05D0AEABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -289,7 +289,7 @@
     <t>C(13,0) V(13,1)</t>
   </si>
   <si>
-    <t>Wilkerbn815</t>
+    <t>Wilkerbn901</t>
   </si>
 </sst>
 </file>

</xml_diff>